<commit_message>
TR-RGR  New  dyanamic Localization as per review changes
</commit_message>
<xml_diff>
--- a/DHL/Template/20230322_ TR_SIR_v8.3.xlsx
+++ b/DHL/Template/20230322_ TR_SIR_v8.3.xlsx
@@ -833,29 +833,29 @@
     <t>ReturnedTax</t>
   </si>
   <si>
-    <t>TypeofCompList</t>
-  </si>
-  <si>
-    <t>IdentificationList</t>
-  </si>
-  <si>
-    <t>IdentityNumImg</t>
-  </si>
-  <si>
-    <t>PassportNumText</t>
-  </si>
-  <si>
-    <t>TexPlateImg</t>
-  </si>
-  <si>
     <t>TaxExceptionConf</t>
+  </si>
+  <si>
+    <t>CompyType</t>
+  </si>
+  <si>
+    <t>IdentyType</t>
+  </si>
+  <si>
+    <t>IdentityCard</t>
+  </si>
+  <si>
+    <t>TurPassportNo</t>
+  </si>
+  <si>
+    <t>TaxPlateImg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +912,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1061,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1142,25 +1154,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,17 +1184,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1614,10 +1632,10 @@
   <dimension ref="A1:AI46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="7" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="5" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,19 +1662,20 @@
     <col min="26" max="26" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="24.140625" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="15" hidden="1" customWidth="1"/>
-    <col min="29" max="30" width="22.85546875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="22.85546875" customWidth="1"/>
     <col min="31" max="32" width="31.42578125" customWidth="1"/>
     <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="45.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="1"/>
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
@@ -1689,78 +1708,78 @@
       <c r="AH1" s="3"/>
     </row>
     <row r="2" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="32" t="s">
         <v>8</v>
       </c>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="S2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="V2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="X2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Y2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="Z2" s="32" t="s">
         <v>18</v>
       </c>
       <c r="AA2" s="37" t="s">
@@ -1769,62 +1788,62 @@
       <c r="AB2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="29" t="s">
+      <c r="AC2" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AD2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="28" t="s">
+      <c r="AE2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="28" t="s">
+      <c r="AF2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="28" t="s">
+      <c r="AG2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
       <c r="AA3" s="37"/>
       <c r="AB3" s="37"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-    </row>
-    <row r="4" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="32"/>
+    </row>
+    <row r="4" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1836,24 +1855,24 @@
       <c r="I4" s="24"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28" t="s">
+      <c r="M4" s="32"/>
+      <c r="N4" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28" t="s">
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28" t="s">
+      <c r="S4" s="32"/>
+      <c r="T4" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="28"/>
+      <c r="U4" s="32"/>
       <c r="V4" s="35" t="s">
         <v>31</v>
       </c>
@@ -1865,14 +1884,14 @@
         <v>33</v>
       </c>
       <c r="Z4" s="36"/>
-      <c r="AA4" s="38" t="s">
+      <c r="AA4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="38" t="s">
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="AD4" s="39"/>
+      <c r="AD4" s="41"/>
       <c r="AE4" s="22" t="s">
         <v>36</v>
       </c>
@@ -1884,7 +1903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2894,7 +2913,7 @@
       <c r="I22" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="J22" s="40"/>
+      <c r="J22" s="28"/>
       <c r="K22" s="19"/>
       <c r="L22" s="20" t="s">
         <v>58</v>
@@ -3292,12 +3311,12 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="41" t="s">
+      <c r="H30" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
       <c r="L30" s="9" t="s">
         <v>144</v>
       </c>
@@ -3346,7 +3365,7 @@
       <c r="G31" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="29" t="s">
         <v>239</v>
       </c>
       <c r="I31" s="19" t="s">
@@ -3403,7 +3422,7 @@
       <c r="G32" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="29" t="s">
         <v>239</v>
       </c>
       <c r="I32" s="19" t="s">
@@ -3458,7 +3477,7 @@
       <c r="G33" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="29" t="s">
         <v>239</v>
       </c>
       <c r="I33" s="19" t="s">
@@ -3513,7 +3532,7 @@
       <c r="G34" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="29" t="s">
         <v>239</v>
       </c>
       <c r="I34" s="19" t="s">
@@ -3626,8 +3645,8 @@
       <c r="I36" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
       <c r="L36" s="20"/>
       <c r="M36" s="14"/>
       <c r="N36" s="20" t="s">
@@ -3673,9 +3692,9 @@
         <v>240</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="J37" s="40"/>
+        <v>242</v>
+      </c>
+      <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="20" t="s">
         <v>198</v>
@@ -3726,9 +3745,9 @@
         <v>240</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="J38" s="40"/>
+        <v>243</v>
+      </c>
+      <c r="J38" s="28"/>
       <c r="K38" s="19"/>
       <c r="L38" s="20" t="s">
         <v>58</v>
@@ -3783,10 +3802,8 @@
       <c r="I39" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="J39" s="28"/>
+      <c r="K39" s="19"/>
       <c r="L39" s="20" t="s">
         <v>66</v>
       </c>
@@ -3838,11 +3855,11 @@
         <v>240</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J40" s="19"/>
       <c r="K40" s="19" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="L40" s="20" t="s">
         <v>74</v>
@@ -3890,12 +3907,12 @@
       <c r="H41" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="I41" s="19" t="s">
-        <v>244</v>
+      <c r="I41" s="42" t="s">
+        <v>245</v>
       </c>
       <c r="J41" s="19"/>
       <c r="K41" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="L41" s="20" t="s">
         <v>81</v>
@@ -3950,9 +3967,9 @@
       <c r="I42" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="J42" s="19"/>
+      <c r="J42" s="43"/>
       <c r="K42" s="19" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="L42" s="20" t="s">
         <v>87</v>
@@ -4005,10 +4022,12 @@
         <v>240</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="K43" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="L43" s="20"/>
       <c r="M43" s="14"/>
       <c r="N43" s="20" t="s">
@@ -4050,12 +4069,11 @@
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="41" t="s">
-        <v>246</v>
-      </c>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
+      <c r="H44" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="9" t="s">
         <v>179</v>
       </c>
@@ -4108,8 +4126,8 @@
       <c r="G45" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="41" t="s">
-        <v>246</v>
+      <c r="H45" s="29" t="s">
+        <v>241</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>227</v>
@@ -4155,8 +4173,8 @@
       <c r="G46" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H46" s="41" t="s">
-        <v>246</v>
+      <c r="H46" s="29" t="s">
+        <v>241</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>226</v>
@@ -4196,11 +4214,11 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AE2:AE3"/>
@@ -4222,10 +4240,6 @@
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -4238,6 +4252,10 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>